<commit_message>
desafio 02 modelo relacional
</commit_message>
<xml_diff>
--- a/Exercicios/Exercicios.xlsx
+++ b/Exercicios/Exercicios.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c49175be73b77308/Área de Trabalho/Programação/BDD/desafio01/Exercicios/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c49175be73b77308/Área de Trabalho/Programação/BDD/Nova pasta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{4A320CD3-C038-4D24-9075-5FFCA078B96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{602D0F81-963B-4F01-ABCF-5EA09DF816BE}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{4A320CD3-C038-4D24-9075-5FFCA078B96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{138C5E56-5362-49B4-9989-896472EBFE30}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FC24E870-CB67-4955-BFC9-DA7A0BA07652}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercicio Rede Social" sheetId="1" r:id="rId1"/>
     <sheet name="Escola" sheetId="2" r:id="rId2"/>
+    <sheet name="Carros" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="168">
   <si>
     <t>tab_postagem</t>
   </si>
@@ -372,12 +373,407 @@
   <si>
     <t xml:space="preserve">CPF , avaliacao_id, notaObtida </t>
   </si>
+  <si>
+    <t>tb_categoria</t>
+  </si>
+  <si>
+    <t>Tb_categoria</t>
+  </si>
+  <si>
+    <r>
+      <t>id,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> descricao, precoDiario</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> modelo, placa , cor, ano, dataAquisicao,</t>
+    </r>
+  </si>
+  <si>
+    <t>id_categoria referencia: tb_categoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> id_categoria, id_sede</t>
+  </si>
+  <si>
+    <t>id_Sede referencia: tb_Sede</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">id, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>logradouro, numero, complemento</t>
+    </r>
+  </si>
+  <si>
+    <t>bairro, cep, id_cidade, id_sede</t>
+  </si>
+  <si>
+    <t>id_cidade referencia: tb_cidade</t>
+  </si>
+  <si>
+    <t>tb_carro</t>
+  </si>
+  <si>
+    <t>tb_sede</t>
+  </si>
+  <si>
+    <t>tb_endereco</t>
+  </si>
+  <si>
+    <t>tb_cidade</t>
+  </si>
+  <si>
+    <t>tb_estado</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">id, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nome, id_estado</t>
+    </r>
+  </si>
+  <si>
+    <t>id_estado referencia tb_estado</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">id, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nome</t>
+    </r>
+  </si>
+  <si>
+    <t>tb_locacao</t>
+  </si>
+  <si>
+    <r>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, instanteLocacao, instanteDevolucao</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+  </si>
+  <si>
+    <t>tb_Cliente</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">cpf, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nome</t>
+    </r>
+  </si>
+  <si>
+    <t>tb_telefone</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t>precoDiario</t>
+  </si>
+  <si>
+    <t>modelo</t>
+  </si>
+  <si>
+    <t>placa</t>
+  </si>
+  <si>
+    <t>cor</t>
+  </si>
+  <si>
+    <t>ano</t>
+  </si>
+  <si>
+    <t>dataAquisicao</t>
+  </si>
+  <si>
+    <t>id_categoria</t>
+  </si>
+  <si>
+    <t>id_sede</t>
+  </si>
+  <si>
+    <t>codigo</t>
+  </si>
+  <si>
+    <t>endereco_id</t>
+  </si>
+  <si>
+    <t>logradouro</t>
+  </si>
+  <si>
+    <t>complement</t>
+  </si>
+  <si>
+    <t>bairro</t>
+  </si>
+  <si>
+    <t>cep</t>
+  </si>
+  <si>
+    <t>cidade_id</t>
+  </si>
+  <si>
+    <t>id_estado</t>
+  </si>
+  <si>
+    <t>instanteLocacao</t>
+  </si>
+  <si>
+    <t>instanteDevolucao</t>
+  </si>
+  <si>
+    <t>tipoLocacao</t>
+  </si>
+  <si>
+    <t>clienteId</t>
+  </si>
+  <si>
+    <t>dias_previstos</t>
+  </si>
+  <si>
+    <t>porcentagemDesconto</t>
+  </si>
+  <si>
+    <t>tb_cliente</t>
+  </si>
+  <si>
+    <t>cliente_id</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>basico</t>
+  </si>
+  <si>
+    <t>polo</t>
+  </si>
+  <si>
+    <t>HDD 9383</t>
+  </si>
+  <si>
+    <t>localidade</t>
+  </si>
+  <si>
+    <t>s:</t>
+  </si>
+  <si>
+    <t>w:</t>
+  </si>
+  <si>
+    <t>local_w</t>
+  </si>
+  <si>
+    <t>local_s</t>
+  </si>
+  <si>
+    <t>Rua flores</t>
+  </si>
+  <si>
+    <t>bloco C</t>
+  </si>
+  <si>
+    <t>Jardim</t>
+  </si>
+  <si>
+    <t>São Paulo</t>
+  </si>
+  <si>
+    <t>fusion</t>
+  </si>
+  <si>
+    <t>luxo</t>
+  </si>
+  <si>
+    <t>PEH3837</t>
+  </si>
+  <si>
+    <t>DIARIA</t>
+  </si>
+  <si>
+    <t>LONGO_PERIODO</t>
+  </si>
+  <si>
+    <t>11/14/2017 09:00</t>
+  </si>
+  <si>
+    <t>maria silva</t>
+  </si>
+  <si>
+    <t>joaquim</t>
+  </si>
+  <si>
+    <t>maria@gmail</t>
+  </si>
+  <si>
+    <t>joaqui@gmail</t>
+  </si>
+  <si>
+    <t>branca: 0</t>
+  </si>
+  <si>
+    <t>preta: 1</t>
+  </si>
+  <si>
+    <t>vermelha: 3</t>
+  </si>
+  <si>
+    <t>cinza: 2</t>
+  </si>
+  <si>
+    <r>
+      <t>codigo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, localidade</t>
+    </r>
+  </si>
+  <si>
+    <t>cpf , numero</t>
+  </si>
+  <si>
+    <t>cpf referencia tab_cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dias_previstos, porcentagemDesconto, </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">tipoLocacao, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cliente_id, localRetirada</t>
+    </r>
+  </si>
+  <si>
+    <t>cliente_id referencia tab_cliente,                          localRetira referencia tb_sede</t>
+  </si>
+  <si>
+    <t>18.28272</t>
+  </si>
+  <si>
+    <t>local_retirada</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,8 +829,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,8 +914,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -578,12 +1045,112 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -609,15 +1176,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -648,6 +1206,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -656,6 +1223,125 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -806,6 +1492,143 @@
         <a:xfrm>
           <a:off x="14253883" y="2077571"/>
           <a:ext cx="6514842" cy="4825775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>246918</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>46859</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1981768-23FD-3DEF-7F31-3ABA0D8DB14D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3695700" y="0"/>
+          <a:ext cx="5857143" cy="6123809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>418370</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>94932</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA96E7F2-3168-FB7B-A14D-8F4874D683A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3886200" y="5934075"/>
+          <a:ext cx="5838095" cy="2542857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>160930</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>123150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagem 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD80B73E-26CC-4852-8617-5DE4072BCA40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18840450" y="171450"/>
+          <a:ext cx="7961905" cy="5400000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1139,22 +1962,22 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
-      <c r="H2" s="9" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+      <c r="H2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="11"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="21"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1340,23 +2163,23 @@
     </row>
     <row r="10" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="H11" s="9" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="H11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="11"/>
-      <c r="N11" s="9" t="s">
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="21"/>
+      <c r="N11" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="O11" s="11"/>
+      <c r="O11" s="21"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
@@ -1571,7 +2394,7 @@
   <dimension ref="B1:T29"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,7 +2407,7 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:20" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="18" t="s">
         <v>43</v>
       </c>
       <c r="O2" s="22" t="s">
@@ -1597,58 +2420,58 @@
       <c r="T2" s="24"/>
     </row>
     <row r="3" spans="2:20" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="P3" s="18" t="s">
+      <c r="O3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="18" t="s">
+      <c r="Q3" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R3" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="S3" s="18" t="s">
+      <c r="S3" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="18" t="s">
+      <c r="T3" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="O4" s="18">
-        <v>1</v>
-      </c>
-      <c r="P4" s="18" t="s">
+      <c r="O4" s="15">
+        <v>1</v>
+      </c>
+      <c r="P4" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="Q4" s="18">
+      <c r="Q4" s="15">
         <v>10</v>
       </c>
-      <c r="R4" s="18">
+      <c r="R4" s="15">
         <v>80</v>
       </c>
-      <c r="S4" s="18">
+      <c r="S4" s="15">
         <v>100</v>
       </c>
-      <c r="T4" s="18">
+      <c r="T4" s="15">
         <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
     </row>
     <row r="6" spans="2:20" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="18" t="s">
         <v>45</v>
       </c>
       <c r="O6" s="22" t="s">
@@ -1660,42 +2483,42 @@
       <c r="S6" s="24"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="O7" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="P7" s="18" t="s">
+      <c r="O7" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="P7" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="Q7" s="18" t="s">
+      <c r="Q7" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="R7" s="18" t="s">
+      <c r="R7" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="S7" s="18" t="s">
+      <c r="S7" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="O8" s="18">
-        <v>1</v>
-      </c>
-      <c r="P8" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="18">
+      <c r="O8" s="15">
+        <v>1</v>
+      </c>
+      <c r="P8" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="15">
         <v>42988</v>
       </c>
-      <c r="R8" s="18">
+      <c r="R8" s="15">
         <v>30</v>
       </c>
-      <c r="S8" s="18">
+      <c r="S8" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1708,51 +2531,51 @@
       <c r="Q10" s="24"/>
     </row>
     <row r="11" spans="2:20" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="O11" s="18" t="s">
+      <c r="O11" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="P11" s="18" t="s">
+      <c r="P11" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="Q11" s="18" t="s">
+      <c r="Q11" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="O12" s="18" t="s">
+      <c r="O12" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="P12" s="18" t="s">
+      <c r="P12" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="Q12" s="20">
+      <c r="Q12" s="17">
         <v>33075</v>
       </c>
     </row>
     <row r="13" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O13" s="18" t="s">
+      <c r="O13" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="P13" s="18" t="s">
+      <c r="P13" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="Q13" s="20">
+      <c r="Q13" s="17">
         <v>33484</v>
       </c>
     </row>
     <row r="14" spans="2:20" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="9" t="s">
         <v>78</v>
       </c>
       <c r="O15" s="22" t="s">
@@ -1762,47 +2585,47 @@
       <c r="Q15" s="24"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="O16" s="18" t="s">
+      <c r="O16" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="P16" s="18" t="s">
+      <c r="P16" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="Q16" s="18" t="s">
+      <c r="Q16" s="15" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="O17" s="18">
-        <v>1</v>
-      </c>
-      <c r="P17" s="18" t="s">
+      <c r="O17" s="15">
+        <v>1</v>
+      </c>
+      <c r="P17" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="Q17" s="18">
+      <c r="Q17" s="15">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="O18" s="18">
-        <v>1</v>
-      </c>
-      <c r="P18" s="18" t="s">
+      <c r="O18" s="15">
+        <v>1</v>
+      </c>
+      <c r="P18" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="Q18" s="18">
+      <c r="Q18" s="15">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="18" t="s">
         <v>51</v>
       </c>
       <c r="O20" s="22" t="s">
@@ -1813,60 +2636,60 @@
       <c r="R20" s="24"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="O21" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="P21" s="18" t="s">
+      <c r="O21" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="P21" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="Q21" s="18" t="s">
+      <c r="Q21" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="R21" s="18" t="s">
+      <c r="R21" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="O22" s="18">
-        <v>1</v>
-      </c>
-      <c r="P22" s="18">
+      <c r="O22" s="15">
+        <v>1</v>
+      </c>
+      <c r="P22" s="15">
         <v>40</v>
       </c>
-      <c r="Q22" s="20">
+      <c r="Q22" s="17">
         <v>43028</v>
       </c>
-      <c r="R22" s="18">
+      <c r="R22" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O23" s="18">
+      <c r="O23" s="15">
         <v>2</v>
       </c>
-      <c r="P23" s="18">
+      <c r="P23" s="15">
         <v>60</v>
       </c>
-      <c r="Q23" s="20">
+      <c r="Q23" s="17">
         <v>43069</v>
       </c>
-      <c r="R23" s="18">
+      <c r="R23" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:18" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="18" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="25" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="9" t="s">
         <v>84</v>
       </c>
       <c r="O25" s="22" t="s">
@@ -1876,52 +2699,52 @@
       <c r="Q25" s="24"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="O26" s="18" t="s">
+      <c r="O26" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="P26" s="18" t="s">
+      <c r="P26" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="Q26" s="18" t="s">
+      <c r="Q26" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="27" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="O27" s="18" t="s">
+      <c r="O27" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="P27" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="18">
+      <c r="P27" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="15">
         <v>35</v>
       </c>
     </row>
     <row r="28" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="O28" s="18" t="s">
+      <c r="O28" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="P28" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="18">
+      <c r="P28" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="15">
         <v>36.5</v>
       </c>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="O29" s="18" t="s">
+      <c r="O29" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="P29" s="18">
+      <c r="P29" s="15">
         <v>2</v>
       </c>
-      <c r="Q29" s="18">
+      <c r="Q29" s="15">
         <v>52.4</v>
       </c>
     </row>
@@ -1938,4 +2761,859 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9CD1D8-891B-4867-9337-16E6FDACEECC}">
+  <dimension ref="B1:W54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:22" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="38"/>
+    </row>
+    <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="O3" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q3" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+    </row>
+    <row r="4" spans="2:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="49">
+        <v>1</v>
+      </c>
+      <c r="P4" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q4" s="51">
+        <v>60</v>
+      </c>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
+      <c r="V4" s="41"/>
+    </row>
+    <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O5" s="49">
+        <v>2</v>
+      </c>
+      <c r="P5" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q5" s="51">
+        <v>150</v>
+      </c>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
+      <c r="V5" s="41"/>
+    </row>
+    <row r="6" spans="2:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="41"/>
+      <c r="V6" s="41"/>
+    </row>
+    <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="41"/>
+      <c r="V7" s="41"/>
+    </row>
+    <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="O8" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="44"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="O9" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="P9" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q9" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="R9" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="S9" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="T9" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="U9" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="V9" s="48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="O10" s="49">
+        <v>1</v>
+      </c>
+      <c r="P10" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q10" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="R10" s="50">
+        <v>0</v>
+      </c>
+      <c r="S10" s="50">
+        <v>2015</v>
+      </c>
+      <c r="T10" s="52">
+        <v>42206</v>
+      </c>
+      <c r="U10" s="50">
+        <v>1</v>
+      </c>
+      <c r="V10" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="49">
+        <v>2</v>
+      </c>
+      <c r="P11" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q11" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="R11" s="63">
+        <v>1</v>
+      </c>
+      <c r="S11" s="50">
+        <v>2016</v>
+      </c>
+      <c r="T11" s="52">
+        <v>42729</v>
+      </c>
+      <c r="U11" s="50">
+        <v>2</v>
+      </c>
+      <c r="V11" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O12" s="1"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="41"/>
+      <c r="V12" s="41"/>
+    </row>
+    <row r="13" spans="2:22" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="O13" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="44"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="O14" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="P14" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q14" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="R14" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+    </row>
+    <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="30"/>
+      <c r="O15" s="49">
+        <v>1</v>
+      </c>
+      <c r="P15" s="50">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="65" t="s">
+        <v>166</v>
+      </c>
+      <c r="R15" s="53">
+        <v>2338474</v>
+      </c>
+      <c r="S15" s="41"/>
+      <c r="T15" s="41"/>
+      <c r="U15" s="41"/>
+      <c r="V15" s="41"/>
+    </row>
+    <row r="16" spans="2:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O16" s="1"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="41"/>
+      <c r="R16" s="41"/>
+      <c r="S16" s="41"/>
+      <c r="T16" s="41"/>
+      <c r="U16" s="41"/>
+      <c r="V16" s="41"/>
+    </row>
+    <row r="17" spans="2:23" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="O17" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="43"/>
+      <c r="S17" s="43"/>
+      <c r="T17" s="43"/>
+      <c r="U17" s="44"/>
+      <c r="V17" s="41"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B18" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="O18" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="P18" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q18" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="R18" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="S18" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="T18" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="U18" s="48" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B19" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="O19" s="49">
+        <v>1</v>
+      </c>
+      <c r="P19" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q19" s="50">
+        <v>205</v>
+      </c>
+      <c r="R19" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="S19" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="T19" s="50">
+        <v>38400282</v>
+      </c>
+      <c r="U19" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B20" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="O20" s="1"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="41"/>
+      <c r="R20" s="41"/>
+      <c r="S20" s="41"/>
+      <c r="T20" s="41"/>
+      <c r="U20" s="41"/>
+      <c r="V20" s="41"/>
+    </row>
+    <row r="21" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="O21" s="1"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="41"/>
+      <c r="S21" s="41"/>
+      <c r="T21" s="41"/>
+      <c r="U21" s="41"/>
+      <c r="V21" s="41"/>
+    </row>
+    <row r="22" spans="2:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O22" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="56"/>
+      <c r="R22" s="41"/>
+      <c r="S22" s="41"/>
+      <c r="T22" s="41"/>
+      <c r="U22" s="41"/>
+      <c r="V22" s="41"/>
+    </row>
+    <row r="23" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O23" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="P23" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q23" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="R23" s="41"/>
+      <c r="S23" s="41"/>
+      <c r="T23" s="41"/>
+      <c r="U23" s="41"/>
+      <c r="V23" s="41"/>
+    </row>
+    <row r="24" spans="2:23" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="O24" s="49">
+        <v>1</v>
+      </c>
+      <c r="P24" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q24" s="53">
+        <v>1</v>
+      </c>
+      <c r="R24" s="41"/>
+      <c r="S24" s="41"/>
+      <c r="T24" s="41"/>
+      <c r="U24" s="41"/>
+      <c r="V24" s="41"/>
+    </row>
+    <row r="25" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="O25" s="1"/>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="41"/>
+      <c r="R25" s="41"/>
+      <c r="S25" s="41"/>
+      <c r="T25" s="41"/>
+      <c r="U25" s="41"/>
+      <c r="V25" s="41"/>
+    </row>
+    <row r="26" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="O26" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="P26" s="44"/>
+      <c r="Q26" s="41"/>
+      <c r="R26" s="41"/>
+      <c r="S26" s="41"/>
+      <c r="T26" s="41"/>
+      <c r="U26" s="41"/>
+      <c r="V26" s="41"/>
+    </row>
+    <row r="27" spans="2:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O27" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="P27" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q27" s="41"/>
+      <c r="R27" s="41"/>
+      <c r="S27" s="41"/>
+      <c r="T27" s="41"/>
+      <c r="U27" s="41"/>
+      <c r="V27" s="41"/>
+    </row>
+    <row r="28" spans="2:23" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="O28" s="49">
+        <v>1</v>
+      </c>
+      <c r="P28" s="53" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q28" s="41"/>
+      <c r="R28" s="41"/>
+      <c r="S28" s="41"/>
+      <c r="T28" s="41"/>
+      <c r="U28" s="41"/>
+      <c r="V28" s="41"/>
+    </row>
+    <row r="29" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="O29" s="1"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="41"/>
+      <c r="R29" s="41"/>
+      <c r="S29" s="41"/>
+      <c r="T29" s="41"/>
+      <c r="U29" s="41"/>
+      <c r="V29" s="41"/>
+    </row>
+    <row r="30" spans="2:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O30" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="P30" s="43"/>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="43"/>
+      <c r="S30" s="43"/>
+      <c r="T30" s="43"/>
+      <c r="U30" s="43"/>
+      <c r="V30" s="44"/>
+    </row>
+    <row r="31" spans="2:23" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="61" t="s">
+        <v>103</v>
+      </c>
+      <c r="O31" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="P31" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q31" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="R31" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="S31" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="T31" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="U31" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="V31" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="W31" s="41"/>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B32" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="O32" s="49">
+        <v>1</v>
+      </c>
+      <c r="P32" s="57">
+        <v>43008.44027777778</v>
+      </c>
+      <c r="Q32" s="57">
+        <v>43012.486111111109</v>
+      </c>
+      <c r="R32" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="S32" s="50">
+        <v>93838673610</v>
+      </c>
+      <c r="T32" s="50">
+        <v>1</v>
+      </c>
+      <c r="U32" s="50">
+        <v>4</v>
+      </c>
+      <c r="V32" s="58">
+        <v>0</v>
+      </c>
+      <c r="W32" s="41"/>
+    </row>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B33" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="O33" s="49">
+        <v>2</v>
+      </c>
+      <c r="P33" s="50" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q33" s="57">
+        <v>43054.416666666664</v>
+      </c>
+      <c r="R33" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="S33" s="50">
+        <v>93838673610</v>
+      </c>
+      <c r="T33" s="50">
+        <v>1</v>
+      </c>
+      <c r="U33" s="50">
+        <v>4</v>
+      </c>
+      <c r="V33" s="58">
+        <v>0</v>
+      </c>
+      <c r="W33" s="41"/>
+    </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B34" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="O34" s="49">
+        <v>3</v>
+      </c>
+      <c r="P34" s="52">
+        <v>43094</v>
+      </c>
+      <c r="Q34" s="52">
+        <v>43312</v>
+      </c>
+      <c r="R34" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="S34" s="50">
+        <v>58236392715</v>
+      </c>
+      <c r="T34" s="50">
+        <v>1</v>
+      </c>
+      <c r="U34" s="50">
+        <f>Q34-P34</f>
+        <v>218</v>
+      </c>
+      <c r="V34" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="W34" s="41"/>
+    </row>
+    <row r="35" spans="2:23" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="O35" s="1"/>
+      <c r="P35" s="41"/>
+      <c r="Q35" s="41"/>
+      <c r="R35" s="41"/>
+      <c r="S35" s="41"/>
+      <c r="T35" s="41"/>
+      <c r="U35" s="41"/>
+      <c r="V35" s="41"/>
+    </row>
+    <row r="36" spans="2:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O36" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="P36" s="43"/>
+      <c r="Q36" s="44"/>
+      <c r="R36" s="41"/>
+      <c r="S36" s="41"/>
+      <c r="T36" s="41"/>
+      <c r="U36" s="41"/>
+      <c r="V36" s="41"/>
+    </row>
+    <row r="37" spans="2:23" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="O37" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="P37" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q37" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="R37" s="41"/>
+      <c r="S37" s="41"/>
+      <c r="T37" s="41"/>
+      <c r="U37" s="41"/>
+      <c r="V37" s="41"/>
+    </row>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B38" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="O38" s="59">
+        <v>93838673610</v>
+      </c>
+      <c r="P38" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q38" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="R38" s="41"/>
+      <c r="S38" s="41"/>
+      <c r="T38" s="41"/>
+      <c r="U38" s="41"/>
+      <c r="V38" s="41"/>
+    </row>
+    <row r="39" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="32"/>
+      <c r="O39" s="59">
+        <v>58236392715</v>
+      </c>
+      <c r="P39" s="50" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q39" s="60" t="s">
+        <v>155</v>
+      </c>
+      <c r="R39" s="41"/>
+      <c r="S39" s="41"/>
+      <c r="T39" s="41"/>
+      <c r="U39" s="41"/>
+      <c r="V39" s="41"/>
+    </row>
+    <row r="40" spans="2:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O40" s="1"/>
+      <c r="P40" s="41"/>
+      <c r="Q40" s="41"/>
+      <c r="R40" s="41"/>
+      <c r="S40" s="41"/>
+      <c r="T40" s="41"/>
+      <c r="U40" s="41"/>
+      <c r="V40" s="41"/>
+    </row>
+    <row r="41" spans="2:23" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="O41" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="P41" s="44"/>
+      <c r="Q41" s="41"/>
+      <c r="R41" s="41"/>
+      <c r="S41" s="41"/>
+      <c r="T41" s="41"/>
+      <c r="U41" s="41"/>
+      <c r="V41" s="41"/>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B42" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="O42" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="P42" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q42" s="41"/>
+      <c r="R42" s="41"/>
+      <c r="S42" s="41"/>
+      <c r="T42" s="41"/>
+      <c r="U42" s="41"/>
+    </row>
+    <row r="43" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="O43" s="59">
+        <v>93838673610</v>
+      </c>
+      <c r="P43" s="53">
+        <v>37635393</v>
+      </c>
+      <c r="Q43" s="41"/>
+      <c r="R43" s="41"/>
+      <c r="S43" s="41"/>
+      <c r="T43" s="41"/>
+      <c r="U43" s="41"/>
+    </row>
+    <row r="44" spans="2:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O44" s="59">
+        <v>58236392715</v>
+      </c>
+      <c r="P44" s="53">
+        <v>37636364</v>
+      </c>
+      <c r="Q44" s="41"/>
+      <c r="R44" s="41"/>
+      <c r="S44" s="41"/>
+      <c r="T44" s="41"/>
+      <c r="U44" s="41"/>
+    </row>
+    <row r="45" spans="2:23" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="61" t="s">
+        <v>137</v>
+      </c>
+      <c r="O45" s="59">
+        <v>58236392715</v>
+      </c>
+      <c r="P45" s="53">
+        <v>89988464</v>
+      </c>
+      <c r="Q45" s="41"/>
+      <c r="R45" s="41"/>
+      <c r="S45" s="41"/>
+      <c r="T45" s="41"/>
+      <c r="U45" s="41"/>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B46" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="U46" s="40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="45" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="2:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="2:2" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="61" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="45" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="O17:U17"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="O13:R13"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O36:Q36"/>
+    <mergeCell ref="O30:V30"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="O8:V8"/>
+    <mergeCell ref="O22:Q22"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="Q38" r:id="rId1" xr:uid="{95FEA5D9-7CA3-48D1-B9F8-5277487923F9}"/>
+    <hyperlink ref="Q39" r:id="rId2" xr:uid="{BEEF66D8-18FF-4BB9-9F2C-D43059FF61DF}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>